<commit_message>
Fixed time and spacing
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -413,215 +413,231 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A4:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Key_f</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Score_f</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Key_t</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Score_t</t>
-        </is>
-      </c>
-    </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Court of Stars</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>20</v>
-      </c>
-      <c r="C3" t="n">
-        <v>171.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v/>
-      </c>
-      <c r="E3" t="n">
-        <v>19</v>
-      </c>
-      <c r="F3" t="n">
-        <v>165</v>
-      </c>
-    </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Halls of Valor</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" t="n">
-        <v>163.1</v>
-      </c>
-      <c r="D4" t="n">
-        <v/>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" t="n">
-        <v>172.6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Temple of the Jade Serpent</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C5" t="n">
-        <v>171.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v/>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F5" t="n">
-        <v>160.1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Shadowmoon Burial Ground</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>20</v>
-      </c>
-      <c r="C6" t="n">
-        <v>174.2</v>
-      </c>
-      <c r="D6" t="n">
-        <v/>
-      </c>
-      <c r="E6" t="n">
-        <v>20</v>
-      </c>
-      <c r="F6" t="n">
-        <v>173.6</v>
+          <t>lilmadman</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>05/04/2023 05:03 PM</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ruby Life Pools</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>20</v>
-      </c>
-      <c r="C7" t="n">
-        <v>170.7</v>
-      </c>
-      <c r="D7" t="n">
-        <v/>
-      </c>
-      <c r="E7" t="n">
-        <v>18</v>
-      </c>
-      <c r="F7" t="n">
-        <v>150.3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Alegthar Academy</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>20</v>
-      </c>
-      <c r="C8" t="n">
-        <v>171</v>
-      </c>
-      <c r="D8" t="n">
-        <v/>
-      </c>
-      <c r="E8" t="n">
-        <v>20</v>
-      </c>
-      <c r="F8" t="n">
-        <v>164.4</v>
-      </c>
-    </row>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Key_f</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Score_f</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Key_t</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Score_t</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Azure Vault</t>
+          <t>Court of Stars</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>164.3</v>
+        <v>171.6</v>
       </c>
       <c r="D9" t="n">
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="n">
-        <v>171.2</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Halls of Valor</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>163.1</v>
+      </c>
+      <c r="D10" t="n">
+        <v/>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>172.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Temple of the Jade Serpent</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>20</v>
+      </c>
+      <c r="C11" t="n">
+        <v>171.5</v>
+      </c>
+      <c r="D11" t="n">
+        <v/>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>160.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Shadowmoon Burial Ground</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>20</v>
+      </c>
+      <c r="C12" t="n">
+        <v>174.2</v>
+      </c>
+      <c r="D12" t="n">
+        <v/>
+      </c>
+      <c r="E12" t="n">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
+        <v>173.6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Ruby Life Pools</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>20</v>
+      </c>
+      <c r="C13" t="n">
+        <v>170.7</v>
+      </c>
+      <c r="D13" t="n">
+        <v/>
+      </c>
+      <c r="E13" t="n">
+        <v>18</v>
+      </c>
+      <c r="F13" t="n">
+        <v>150.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Alegthar Academy</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" t="n">
+        <v>171</v>
+      </c>
+      <c r="D14" t="n">
+        <v/>
+      </c>
+      <c r="E14" t="n">
+        <v>20</v>
+      </c>
+      <c r="F14" t="n">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Azure Vault</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" t="n">
+        <v>164.3</v>
+      </c>
+      <c r="D15" t="n">
+        <v/>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+      <c r="F15" t="n">
+        <v>171.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Nokund Offensive</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>20</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B16" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" t="n">
         <v>170.7</v>
       </c>
-      <c r="D10" t="n">
-        <v/>
-      </c>
-      <c r="E10" t="n">
-        <v>20</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="D16" t="n">
+        <v/>
+      </c>
+      <c r="E16" t="n">
+        <v>20</v>
+      </c>
+      <c r="F16" t="n">
         <v>170.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add dungeons needed to work on; added formatting; started functions for calculation
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A4:F16"/>
+  <dimension ref="A4:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,18 +426,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lilmadman</t>
+          <t>lilmadman   2716</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/04/2023 05:03 PM</t>
+          <t>05/05/2023 11:54 AM</t>
         </is>
       </c>
     </row>
@@ -639,6 +643,84 @@
       </c>
       <c r="F16" t="n">
         <v>170.8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Fortified Need</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>Tyrannical Need</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="n"/>
+      <c r="F18" s="1" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Halls of Valor</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v/>
+      </c>
+      <c r="C19" t="n">
+        <v/>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Ruby Life Pools</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Azure Vault</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v/>
+      </c>
+      <c r="C20" t="n">
+        <v/>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Temple of the Jade Serpent</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ruby Life Pools</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v/>
+      </c>
+      <c r="C21" t="n">
+        <v/>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Alegthar Academy</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted for new key names
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -437,7 +437,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/05/2023 11:54 AM</t>
+          <t>05/08/2023 04:41 PM</t>
         </is>
       </c>
     </row>
@@ -472,29 +472,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Court of Stars</t>
+          <t>Brackenhide Hold</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>171.6</v>
+        <v>174.2</v>
       </c>
       <c r="D9" t="n">
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" t="n">
-        <v>165</v>
+        <v>173.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Halls of Valor</t>
+          <t>Halls of Infusion</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -516,36 +516,36 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Temple of the Jade Serpent</t>
+          <t>Neltharus</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>20</v>
       </c>
       <c r="C11" t="n">
-        <v>171.5</v>
+        <v>171.6</v>
       </c>
       <c r="D11" t="n">
         <v/>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>160.1</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Shadowmoon Burial Ground</t>
+          <t>Uldaman: Legacy of Tyr</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>174.2</v>
+        <v>171.5</v>
       </c>
       <c r="D12" t="n">
         <v/>
@@ -554,35 +554,35 @@
         <v>20</v>
       </c>
       <c r="F12" t="n">
-        <v>173.6</v>
+        <v>160.1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ruby Life Pools</t>
+          <t>Freehold</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>20</v>
       </c>
       <c r="C13" t="n">
-        <v>170.7</v>
+        <v>164.3</v>
       </c>
       <c r="D13" t="n">
         <v/>
       </c>
       <c r="E13" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" t="n">
-        <v>150.3</v>
+        <v>171.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Alegthar Academy</t>
+          <t>Neltharion's Lair</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -604,14 +604,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Azure Vault</t>
+          <t>The Underrot</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>20</v>
       </c>
       <c r="C15" t="n">
-        <v>164.3</v>
+        <v>170.7</v>
       </c>
       <c r="D15" t="n">
         <v/>
@@ -620,13 +620,13 @@
         <v>20</v>
       </c>
       <c r="F15" t="n">
-        <v>171.2</v>
+        <v>170.8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nokund Offensive</t>
+          <t>The Vortex Pinnacle</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -639,10 +639,10 @@
         <v/>
       </c>
       <c r="E16" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F16" t="n">
-        <v>170.8</v>
+        <v>150.3</v>
       </c>
     </row>
     <row r="18">
@@ -672,7 +672,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Halls of Valor</t>
+          <t>Halls of Infusion</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -683,14 +683,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Ruby Life Pools</t>
+          <t>The Vortex Pinnacle</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Azure Vault</t>
+          <t>Freehold</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -701,14 +701,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Temple of the Jade Serpent</t>
+          <t>Uldaman: Legacy of Tyr</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ruby Life Pools</t>
+          <t>The Underrot</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -719,7 +719,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Alegthar Academy</t>
+          <t>Neltharion's Lair</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed logic of three dungeons and posted to spreadsheet
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A4:F21"/>
+  <dimension ref="A4:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,8 +425,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="4">
@@ -437,7 +437,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/08/2023 04:41 PM</t>
+          <t>05/09/2023 01:44 PM</t>
         </is>
       </c>
     </row>
@@ -720,6 +720,126 @@
       <c r="D21" t="inlineStr">
         <is>
           <t>Neltharion's Lair</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Single Dungeon to reach 2800 -Fort</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>Single Dungeon to reach 2800 -Tyr</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="n"/>
+      <c r="F23" s="1" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Too High of a Key, 31 or Higher</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v/>
+      </c>
+      <c r="C24" t="n">
+        <v/>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Too High of a Key, 31 or Higher</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Three Dungeons to reach 2800 -Fort</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>  </t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Three Dungeons to reach 2800 -Tyr</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="n"/>
+      <c r="F26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Halls of Infusion(24)</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v/>
+      </c>
+      <c r="C27" t="n">
+        <v/>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>The Vortex Pinnacle(22)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Freehold(24)</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v/>
+      </c>
+      <c r="C28" t="n">
+        <v/>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Uldaman: Legacy of Tyr(23)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Brackenhide Hold(25)</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v/>
+      </c>
+      <c r="C29" t="n">
+        <v/>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Neltharus(24)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added conditional get request when ready for live
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -432,12 +432,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lilmadman   2716</t>
+          <t>lilmadman   2745.8</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/09/2023 01:44 PM</t>
+          <t>05/09/2023 01:56 PM</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Too High of a Key, 31 or Higher</t>
+          <t>Halls of Infusion(27)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Too High of a Key, 31 or Higher</t>
+          <t>The Vortex Pinnacle(25)</t>
         </is>
       </c>
     </row>
@@ -792,7 +792,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Halls of Infusion(24)</t>
+          <t>Halls of Infusion(22)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -803,14 +803,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle(22)</t>
+          <t>The Vortex Pinnacle(20)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Freehold(24)</t>
+          <t>Freehold(22)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -821,14 +821,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Uldaman: Legacy of Tyr(23)</t>
+          <t>Uldaman: Legacy of Tyr(22)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(25)</t>
+          <t>Neltharus(23)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -839,7 +839,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Neltharus(24)</t>
+          <t>Neltharion's Lair(22)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Calculator now accounts for empty keys; replaced 'Too High of Key' with +30
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -432,12 +432,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lilmadman   2745.8</t>
+          <t>maddusmaxxus   858.6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/09/2023 01:56 PM</t>
+          <t>05/10/2023 03:55 PM</t>
         </is>
       </c>
     </row>
@@ -476,19 +476,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>174.2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F9" t="n">
-        <v>173.6</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="10">
@@ -498,19 +498,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>163.1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v/>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F10" t="n">
-        <v>172.6</v>
+        <v>101.7</v>
       </c>
     </row>
     <row r="11">
@@ -520,19 +520,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>171.6</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v/>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F11" t="n">
-        <v>165</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
@@ -542,19 +542,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>171.5</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v/>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F12" t="n">
-        <v>160.1</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
@@ -564,19 +564,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>164.3</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v/>
       </c>
       <c r="E13" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F13" t="n">
-        <v>171.2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
@@ -586,19 +586,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v/>
       </c>
       <c r="E14" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F14" t="n">
-        <v>164.4</v>
+        <v>86.40000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>170.7</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v/>
       </c>
       <c r="E15" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>170.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -630,19 +630,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>170.7</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v/>
       </c>
       <c r="E16" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>150.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -672,7 +672,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Halls of Infusion</t>
+          <t>Brackenhide Hold</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -683,14 +683,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle</t>
+          <t>The Underrot</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Freehold</t>
+          <t>Halls of Infusion</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -701,14 +701,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Uldaman: Legacy of Tyr</t>
+          <t>The Vortex Pinnacle</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>The Underrot</t>
+          <t>Neltharus</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -719,14 +719,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Neltharion's Lair</t>
+          <t>Freehold</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 2800 -Fort</t>
+          <t>Single Dungeon to reach 1500 -Fort</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 2800 -Tyr</t>
+          <t>Single Dungeon to reach 1500 -Tyr</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -750,7 +750,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Halls of Infusion(27)</t>
+          <t>Brackenhide Hold(30)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -761,14 +761,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle(25)</t>
+          <t>Brackenhide Hold(30)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 2800 -Fort</t>
+          <t>Three Dungeons to reach 1500 -Fort</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 2800 -Tyr</t>
+          <t>Three Dungeons to reach 1500 -Tyr</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -792,7 +792,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Halls of Infusion(22)</t>
+          <t>Brackenhide Hold(27)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -803,14 +803,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle(20)</t>
+          <t>The Underrot(27)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Freehold(22)</t>
+          <t>Halls of Infusion(27)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -821,14 +821,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Uldaman: Legacy of Tyr(22)</t>
+          <t>The Vortex Pinnacle(27)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Neltharus(23)</t>
+          <t>Neltharus(27)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -839,7 +839,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Neltharion's Lair(22)</t>
+          <t>Brackenhide Hold(30)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added arguments for CLI run
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -432,12 +432,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>maddusmaxxus   858.6</t>
+          <t>valamarth   1600.9</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/10/2023 03:55 PM</t>
+          <t>05/17/2023 12:59 PM</t>
         </is>
       </c>
     </row>
@@ -485,10 +485,10 @@
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" t="n">
-        <v>95.3</v>
+        <v>130.5</v>
       </c>
     </row>
     <row r="10">
@@ -507,10 +507,10 @@
         <v/>
       </c>
       <c r="E10" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F10" t="n">
-        <v>101.7</v>
+        <v>142.8</v>
       </c>
     </row>
     <row r="11">
@@ -529,10 +529,10 @@
         <v/>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F11" t="n">
-        <v>102</v>
+        <v>136.4</v>
       </c>
     </row>
     <row r="12">
@@ -551,10 +551,10 @@
         <v/>
       </c>
       <c r="E12" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" t="n">
-        <v>102</v>
+        <v>129.2</v>
       </c>
     </row>
     <row r="13">
@@ -573,10 +573,10 @@
         <v/>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F13" t="n">
-        <v>85</v>
+        <v>143.2</v>
       </c>
     </row>
     <row r="14">
@@ -595,10 +595,10 @@
         <v/>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F14" t="n">
-        <v>86.40000000000001</v>
+        <v>108.6</v>
       </c>
     </row>
     <row r="15">
@@ -617,10 +617,10 @@
         <v/>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>132.4</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         <v/>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>144.3</v>
       </c>
     </row>
     <row r="18">
@@ -683,7 +683,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>The Underrot</t>
+          <t>Neltharion's Lair</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle</t>
+          <t>Uldaman: Legacy of Tyr</t>
         </is>
       </c>
     </row>
@@ -719,14 +719,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Freehold</t>
+          <t>Brackenhide Hold</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 1500 -Fort</t>
+          <t>Single Dungeon to reach 2000 -Fort</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 1500 -Tyr</t>
+          <t>Single Dungeon to reach 2000 -Tyr</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -768,7 +768,7 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 1500 -Fort</t>
+          <t>Three Dungeons to reach 2000 -Fort</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 1500 -Tyr</t>
+          <t>Three Dungeons to reach 2000 -Tyr</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -792,7 +792,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(27)</t>
+          <t>Brackenhide Hold(15)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -803,14 +803,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>The Underrot(27)</t>
+          <t>Brackenhide Hold(30)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Halls of Infusion(27)</t>
+          <t>Halls of Infusion(15)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -821,14 +821,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>The Vortex Pinnacle(27)</t>
+          <t>Halls of Infusion(30)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Neltharus(27)</t>
+          <t>Neltharus(15)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -839,7 +839,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(30)</t>
+          <t>Neltharus(30)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2800, and 3000 as goals
</commit_message>
<xml_diff>
--- a/dungeon.xlsx
+++ b/dungeon.xlsx
@@ -432,12 +432,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>valamarth   1600.9</t>
+          <t>maddusmaxxus   2438.6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>05/17/2023 12:59 PM</t>
+          <t>05/30/2023 02:34 PM</t>
         </is>
       </c>
     </row>
@@ -476,19 +476,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>146.4</v>
       </c>
       <c r="D9" t="n">
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F9" t="n">
-        <v>130.5</v>
+        <v>158.3</v>
       </c>
     </row>
     <row r="10">
@@ -498,10 +498,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>144.9</v>
       </c>
       <c r="D10" t="n">
         <v/>
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="n">
-        <v>142.8</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="11">
@@ -520,19 +520,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>142.5</v>
       </c>
       <c r="D11" t="n">
         <v/>
       </c>
       <c r="E11" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>136.4</v>
+        <v>153.7</v>
       </c>
     </row>
     <row r="12">
@@ -542,19 +542,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>142.6</v>
       </c>
       <c r="D12" t="n">
         <v/>
       </c>
       <c r="E12" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F12" t="n">
-        <v>129.2</v>
+        <v>150.7</v>
       </c>
     </row>
     <row r="13">
@@ -564,19 +564,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>149.5</v>
       </c>
       <c r="D13" t="n">
         <v/>
       </c>
       <c r="E13" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F13" t="n">
-        <v>143.2</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="14">
@@ -586,19 +586,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>137.9</v>
       </c>
       <c r="D14" t="n">
         <v/>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F14" t="n">
-        <v>108.6</v>
+        <v>150.8</v>
       </c>
     </row>
     <row r="15">
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>151.5</v>
       </c>
       <c r="D15" t="n">
         <v/>
       </c>
       <c r="E15" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F15" t="n">
-        <v>132.4</v>
+        <v>151.9</v>
       </c>
     </row>
     <row r="16">
@@ -630,19 +630,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="D16" t="n">
         <v/>
       </c>
       <c r="E16" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F16" t="n">
-        <v>144.3</v>
+        <v>164.3</v>
       </c>
     </row>
     <row r="18">
@@ -672,7 +672,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brackenhide Hold</t>
+          <t>Neltharion's Lair</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -683,14 +683,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Neltharion's Lair</t>
+          <t>Halls of Infusion</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Halls of Infusion</t>
+          <t>Neltharus</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -708,7 +708,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Neltharus</t>
+          <t>Uldaman: Legacy of Tyr</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -719,14 +719,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Brackenhide Hold</t>
+          <t>Neltharion's Lair</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 2000 -Fort</t>
+          <t>Single Dungeon to reach 2500 -Fort</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>Single Dungeon to reach 2000 -Tyr</t>
+          <t>Single Dungeon to reach 2500 -Tyr</t>
         </is>
       </c>
       <c r="E23" s="1" t="n"/>
@@ -750,7 +750,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(30)</t>
+          <t>Neltharus(25)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -761,14 +761,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(30)</t>
+          <t>Halls of Infusion(26)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 2000 -Fort</t>
+          <t>Three Dungeons to reach 2500 -Fort</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>Three Dungeons to reach 2000 -Tyr</t>
+          <t>Three Dungeons to reach 2500 -Tyr</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -792,7 +792,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(15)</t>
+          <t>Neltharion's Lair(19)</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -803,14 +803,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Brackenhide Hold(30)</t>
+          <t>Halls of Infusion(21)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Halls of Infusion(15)</t>
+          <t>Brackenhide Hold(20)</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -821,14 +821,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Halls of Infusion(30)</t>
+          <t>Neltharus(21)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Neltharus(15)</t>
+          <t>Halls of Infusion(20)</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -839,7 +839,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Neltharus(30)</t>
+          <t>Uldaman: Legacy of Tyr(21)</t>
         </is>
       </c>
     </row>

</xml_diff>